<commit_message>
Update Theo dõi công nợ Thanh Hà.xlsx
</commit_message>
<xml_diff>
--- a/KẾ TOÁN - THÁI HẰNG/CÔNG NỢ/THANH HÀ/Theo dõi công nợ Thanh Hà.xlsx
+++ b/KẾ TOÁN - THÁI HẰNG/CÔNG NỢ/THANH HÀ/Theo dõi công nợ Thanh Hà.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="40">
   <si>
     <t>CÔNG TY CỔ PHẦN ĐT &amp; PT NANO MILK</t>
   </si>
@@ -147,10 +147,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0\ _₫_-;\-* #,##0\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0\ _₫_-;\-* #,##0\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -248,7 +248,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -412,42 +412,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="205">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -456,25 +469,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -483,7 +496,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -492,19 +505,19 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -513,7 +526,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -525,7 +538,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -537,7 +550,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -546,10 +559,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -558,22 +568,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -582,7 +592,7 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -611,57 +621,54 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -673,14 +680,189 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -694,13 +876,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -715,10 +897,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -736,7 +918,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -745,6 +927,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -754,15 +942,36 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -784,50 +993,29 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1111,116 +1299,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="59" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="59" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="59" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="59" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="59"/>
-    <col min="6" max="6" width="9.28515625" style="59" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="59" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" style="59" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" style="59" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" style="59" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.42578125" style="59" customWidth="1"/>
-    <col min="12" max="12" width="4.140625" style="59" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" style="59" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="59"/>
+    <col min="1" max="1" width="4.85546875" style="58" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="58" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="58" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="58" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="58"/>
+    <col min="6" max="6" width="9.28515625" style="58" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="58" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" style="58" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" style="58" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" style="58" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.42578125" style="58" customWidth="1"/>
+    <col min="12" max="12" width="4.140625" style="58" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" style="58" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="58"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="57"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="56"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="62"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="61"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
     </row>
     <row r="3" spans="1:17" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="114" t="s">
+      <c r="A3" s="177" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="114"/>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114"/>
-      <c r="H3" s="114"/>
-      <c r="I3" s="114"/>
-      <c r="J3" s="114"/>
-      <c r="K3" s="114"/>
-      <c r="L3" s="114"/>
-      <c r="M3" s="114"/>
-      <c r="N3" s="114"/>
-      <c r="O3" s="114"/>
-      <c r="P3" s="114"/>
-      <c r="Q3" s="114"/>
+      <c r="B3" s="177"/>
+      <c r="C3" s="177"/>
+      <c r="D3" s="177"/>
+      <c r="E3" s="177"/>
+      <c r="F3" s="177"/>
+      <c r="G3" s="177"/>
+      <c r="H3" s="177"/>
+      <c r="I3" s="177"/>
+      <c r="J3" s="177"/>
+      <c r="K3" s="177"/>
+      <c r="L3" s="177"/>
+      <c r="M3" s="177"/>
+      <c r="N3" s="177"/>
+      <c r="O3" s="177"/>
+      <c r="P3" s="177"/>
+      <c r="Q3" s="177"/>
     </row>
     <row r="5" spans="1:17" s="21" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="115" t="s">
+      <c r="A5" s="178" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="117" t="s">
+      <c r="B5" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="119" t="s">
+      <c r="C5" s="182" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="119"/>
-      <c r="E5" s="96" t="s">
+      <c r="D5" s="182"/>
+      <c r="E5" s="157" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="96"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="96"/>
-      <c r="I5" s="96"/>
-      <c r="J5" s="97" t="s">
+      <c r="F5" s="157"/>
+      <c r="G5" s="157"/>
+      <c r="H5" s="157"/>
+      <c r="I5" s="157"/>
+      <c r="J5" s="158" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="99" t="s">
+      <c r="K5" s="160" t="s">
         <v>36</v>
       </c>
-      <c r="L5" s="99"/>
-      <c r="M5" s="99"/>
-      <c r="N5" s="100" t="s">
+      <c r="L5" s="160"/>
+      <c r="M5" s="160"/>
+      <c r="N5" s="161" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:17" s="21" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="116"/>
-      <c r="B6" s="118"/>
+      <c r="A6" s="179"/>
+      <c r="B6" s="181"/>
       <c r="C6" s="24" t="s">
         <v>21</v>
       </c>
@@ -1242,7 +1430,7 @@
       <c r="I6" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="98"/>
+      <c r="J6" s="159"/>
       <c r="K6" s="22" t="s">
         <v>37</v>
       </c>
@@ -1252,19 +1440,19 @@
       <c r="M6" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="N6" s="101"/>
+      <c r="N6" s="162"/>
     </row>
     <row r="7" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="102">
+      <c r="A7" s="163">
         <v>571</v>
       </c>
-      <c r="B7" s="104">
+      <c r="B7" s="165">
         <v>43990</v>
       </c>
-      <c r="C7" s="108" t="s">
+      <c r="C7" s="169" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="108" t="s">
+      <c r="D7" s="169" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -1297,10 +1485,10 @@
       <c r="P7" s="6"/>
     </row>
     <row r="8" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="110"/>
-      <c r="B8" s="111"/>
-      <c r="C8" s="113"/>
-      <c r="D8" s="113"/>
+      <c r="A8" s="171"/>
+      <c r="B8" s="172"/>
+      <c r="C8" s="174"/>
+      <c r="D8" s="174"/>
       <c r="E8" s="7" t="s">
         <v>7</v>
       </c>
@@ -1330,10 +1518,10 @@
       <c r="N8" s="7"/>
     </row>
     <row r="9" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="110"/>
-      <c r="B9" s="111"/>
-      <c r="C9" s="113"/>
-      <c r="D9" s="113"/>
+      <c r="A9" s="171"/>
+      <c r="B9" s="172"/>
+      <c r="C9" s="174"/>
+      <c r="D9" s="174"/>
       <c r="E9" s="7" t="s">
         <v>8</v>
       </c>
@@ -1363,10 +1551,10 @@
       <c r="N9" s="7"/>
     </row>
     <row r="10" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="110"/>
-      <c r="B10" s="111"/>
-      <c r="C10" s="113"/>
-      <c r="D10" s="113"/>
+      <c r="A10" s="171"/>
+      <c r="B10" s="172"/>
+      <c r="C10" s="174"/>
+      <c r="D10" s="174"/>
       <c r="E10" s="7" t="s">
         <v>9</v>
       </c>
@@ -1396,10 +1584,10 @@
       <c r="N10" s="7"/>
     </row>
     <row r="11" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="110"/>
-      <c r="B11" s="111"/>
-      <c r="C11" s="113"/>
-      <c r="D11" s="113"/>
+      <c r="A11" s="171"/>
+      <c r="B11" s="172"/>
+      <c r="C11" s="174"/>
+      <c r="D11" s="174"/>
       <c r="E11" s="7" t="s">
         <v>10</v>
       </c>
@@ -1429,10 +1617,10 @@
       <c r="N11" s="7"/>
     </row>
     <row r="12" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="110"/>
-      <c r="B12" s="111"/>
-      <c r="C12" s="113"/>
-      <c r="D12" s="113"/>
+      <c r="A12" s="171"/>
+      <c r="B12" s="172"/>
+      <c r="C12" s="174"/>
+      <c r="D12" s="174"/>
       <c r="E12" s="7" t="s">
         <v>11</v>
       </c>
@@ -1462,10 +1650,10 @@
       <c r="N12" s="7"/>
     </row>
     <row r="13" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="110"/>
-      <c r="B13" s="111"/>
-      <c r="C13" s="113"/>
-      <c r="D13" s="113"/>
+      <c r="A13" s="171"/>
+      <c r="B13" s="172"/>
+      <c r="C13" s="174"/>
+      <c r="D13" s="174"/>
       <c r="E13" s="7" t="s">
         <v>12</v>
       </c>
@@ -1495,10 +1683,10 @@
       <c r="N13" s="11"/>
     </row>
     <row r="14" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="103"/>
-      <c r="B14" s="105"/>
-      <c r="C14" s="109"/>
-      <c r="D14" s="109"/>
+      <c r="A14" s="164"/>
+      <c r="B14" s="166"/>
+      <c r="C14" s="170"/>
+      <c r="D14" s="170"/>
       <c r="E14" s="12" t="s">
         <v>13</v>
       </c>
@@ -1528,16 +1716,16 @@
       <c r="N14" s="12"/>
     </row>
     <row r="15" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="102">
+      <c r="A15" s="163">
         <v>587</v>
       </c>
-      <c r="B15" s="104">
+      <c r="B15" s="165">
         <v>43995</v>
       </c>
-      <c r="C15" s="106" t="s">
+      <c r="C15" s="167" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="108" t="s">
+      <c r="D15" s="169" t="s">
         <v>5</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -1570,10 +1758,10 @@
       <c r="O15" s="6"/>
     </row>
     <row r="16" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="103"/>
-      <c r="B16" s="105"/>
-      <c r="C16" s="107"/>
-      <c r="D16" s="109"/>
+      <c r="A16" s="164"/>
+      <c r="B16" s="166"/>
+      <c r="C16" s="168"/>
+      <c r="D16" s="170"/>
       <c r="E16" s="12" t="s">
         <v>14</v>
       </c>
@@ -1603,17 +1791,17 @@
       <c r="N16" s="12"/>
       <c r="O16" s="6"/>
     </row>
-    <row r="17" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="102">
+    <row r="17" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="163">
         <v>479</v>
       </c>
-      <c r="B17" s="104">
+      <c r="B17" s="165">
         <v>43996</v>
       </c>
-      <c r="C17" s="106" t="s">
+      <c r="C17" s="167" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="108" t="s">
+      <c r="D17" s="169" t="s">
         <v>5</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -1645,11 +1833,11 @@
       <c r="N17" s="1"/>
       <c r="O17" s="6"/>
     </row>
-    <row r="18" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="110"/>
-      <c r="B18" s="111"/>
-      <c r="C18" s="112"/>
-      <c r="D18" s="113"/>
+    <row r="18" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="171"/>
+      <c r="B18" s="172"/>
+      <c r="C18" s="173"/>
+      <c r="D18" s="174"/>
       <c r="E18" s="7" t="s">
         <v>14</v>
       </c>
@@ -1679,11 +1867,11 @@
       <c r="N18" s="7"/>
       <c r="O18" s="6"/>
     </row>
-    <row r="19" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="110"/>
-      <c r="B19" s="111"/>
-      <c r="C19" s="112"/>
-      <c r="D19" s="113"/>
+    <row r="19" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="171"/>
+      <c r="B19" s="172"/>
+      <c r="C19" s="173"/>
+      <c r="D19" s="174"/>
       <c r="E19" s="7" t="s">
         <v>11</v>
       </c>
@@ -1713,11 +1901,11 @@
       <c r="N19" s="7"/>
       <c r="O19" s="6"/>
     </row>
-    <row r="20" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="110"/>
-      <c r="B20" s="111"/>
-      <c r="C20" s="112"/>
-      <c r="D20" s="113"/>
+    <row r="20" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="171"/>
+      <c r="B20" s="172"/>
+      <c r="C20" s="173"/>
+      <c r="D20" s="174"/>
       <c r="E20" s="7" t="s">
         <v>15</v>
       </c>
@@ -1747,11 +1935,11 @@
       <c r="N20" s="7"/>
       <c r="O20" s="6"/>
     </row>
-    <row r="21" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="103"/>
-      <c r="B21" s="105"/>
-      <c r="C21" s="107"/>
-      <c r="D21" s="109"/>
+    <row r="21" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="164"/>
+      <c r="B21" s="166"/>
+      <c r="C21" s="168"/>
+      <c r="D21" s="170"/>
       <c r="E21" s="12" t="s">
         <v>16</v>
       </c>
@@ -1781,7 +1969,7 @@
       <c r="N21" s="12"/>
       <c r="O21" s="6"/>
     </row>
-    <row r="22" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <v>597</v>
       </c>
@@ -1820,25 +2008,25 @@
         <f t="shared" si="3"/>
         <v>13650000</v>
       </c>
-      <c r="N22" s="75"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="102">
+      <c r="N22" s="73"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="163">
         <v>635</v>
       </c>
-      <c r="B23" s="104">
+      <c r="B23" s="165">
         <v>44047</v>
       </c>
-      <c r="C23" s="141" t="s">
+      <c r="C23" s="175" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="141" t="s">
+      <c r="D23" s="175" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="87" t="s">
+      <c r="E23" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="87">
+      <c r="F23" s="85">
         <v>24</v>
       </c>
       <c r="G23" s="2">
@@ -1861,19 +2049,19 @@
         <f t="shared" si="3"/>
         <v>5460000</v>
       </c>
-      <c r="N23" s="87"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="103"/>
-      <c r="B24" s="105"/>
-      <c r="C24" s="142"/>
-      <c r="D24" s="142" t="s">
+      <c r="N23" s="85"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="164"/>
+      <c r="B24" s="166"/>
+      <c r="C24" s="176"/>
+      <c r="D24" s="176" t="s">
         <v>5</v>
       </c>
-      <c r="E24" s="89" t="s">
+      <c r="E24" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="89">
+      <c r="F24" s="87">
         <v>24</v>
       </c>
       <c r="G24" s="13">
@@ -1896,25 +2084,25 @@
         <f t="shared" si="3"/>
         <v>5580000</v>
       </c>
-      <c r="N24" s="89"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="102">
+      <c r="N24" s="87"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="163">
         <v>763</v>
       </c>
-      <c r="B25" s="135">
+      <c r="B25" s="183">
         <v>44063</v>
       </c>
-      <c r="C25" s="141" t="s">
+      <c r="C25" s="175" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="141" t="s">
+      <c r="D25" s="175" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="136" t="s">
+      <c r="E25" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="F25" s="87">
+      <c r="F25" s="85">
         <v>48</v>
       </c>
       <c r="G25" s="2">
@@ -1931,25 +2119,25 @@
         <f t="shared" si="1"/>
         <v>5400000</v>
       </c>
-      <c r="K25" s="136"/>
-      <c r="L25" s="136"/>
+      <c r="K25" s="93"/>
+      <c r="L25" s="93"/>
       <c r="M25" s="2">
         <f t="shared" si="3"/>
         <v>5400000</v>
       </c>
-      <c r="N25" s="136"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="110"/>
-      <c r="B26" s="137"/>
-      <c r="C26" s="143"/>
-      <c r="D26" s="143" t="s">
+      <c r="N25" s="93"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="171"/>
+      <c r="B26" s="184"/>
+      <c r="C26" s="186"/>
+      <c r="D26" s="186" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="138" t="s">
+      <c r="E26" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="88">
+      <c r="F26" s="86">
         <v>36</v>
       </c>
       <c r="G26" s="8">
@@ -1966,25 +2154,25 @@
         <f t="shared" si="1"/>
         <v>8190000</v>
       </c>
-      <c r="K26" s="138"/>
-      <c r="L26" s="138"/>
+      <c r="K26" s="94"/>
+      <c r="L26" s="94"/>
       <c r="M26" s="8">
         <f t="shared" si="3"/>
         <v>8190000</v>
       </c>
-      <c r="N26" s="138"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="103"/>
-      <c r="B27" s="139"/>
-      <c r="C27" s="142"/>
-      <c r="D27" s="142" t="s">
+      <c r="N26" s="94"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="164"/>
+      <c r="B27" s="185"/>
+      <c r="C27" s="176"/>
+      <c r="D27" s="176" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="140" t="s">
+      <c r="E27" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="F27" s="89">
+      <c r="F27" s="87">
         <v>36</v>
       </c>
       <c r="G27" s="13">
@@ -2001,31 +2189,31 @@
         <f t="shared" si="1"/>
         <v>8730000</v>
       </c>
-      <c r="K27" s="140"/>
-      <c r="L27" s="140"/>
+      <c r="K27" s="95"/>
+      <c r="L27" s="95"/>
       <c r="M27" s="13">
         <f t="shared" si="3"/>
         <v>8730000</v>
       </c>
-      <c r="N27" s="140"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="102">
+      <c r="N27" s="95"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="163">
         <v>764</v>
       </c>
-      <c r="B28" s="135">
+      <c r="B28" s="183">
         <v>44065</v>
       </c>
-      <c r="C28" s="141" t="s">
+      <c r="C28" s="175" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="141" t="s">
+      <c r="D28" s="175" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="136" t="s">
+      <c r="E28" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="87">
+      <c r="F28" s="85">
         <v>12</v>
       </c>
       <c r="G28" s="2">
@@ -2042,25 +2230,25 @@
         <f t="shared" si="1"/>
         <v>2730000</v>
       </c>
-      <c r="K28" s="136"/>
-      <c r="L28" s="136"/>
+      <c r="K28" s="93"/>
+      <c r="L28" s="93"/>
       <c r="M28" s="2">
         <f t="shared" si="3"/>
         <v>2730000</v>
       </c>
-      <c r="N28" s="136"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="110"/>
-      <c r="B29" s="137"/>
-      <c r="C29" s="143"/>
-      <c r="D29" s="143" t="s">
+      <c r="N28" s="93"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="171"/>
+      <c r="B29" s="184"/>
+      <c r="C29" s="186"/>
+      <c r="D29" s="186" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="138" t="s">
+      <c r="E29" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="88">
+      <c r="F29" s="86">
         <v>60</v>
       </c>
       <c r="G29" s="8">
@@ -2077,25 +2265,25 @@
         <f t="shared" si="1"/>
         <v>13950000</v>
       </c>
-      <c r="K29" s="138"/>
-      <c r="L29" s="138"/>
+      <c r="K29" s="94"/>
+      <c r="L29" s="94"/>
       <c r="M29" s="8">
         <f t="shared" si="3"/>
         <v>13950000</v>
       </c>
-      <c r="N29" s="138"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="110"/>
-      <c r="B30" s="137"/>
-      <c r="C30" s="143"/>
-      <c r="D30" s="143" t="s">
+      <c r="N29" s="94"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="171"/>
+      <c r="B30" s="184"/>
+      <c r="C30" s="186"/>
+      <c r="D30" s="186" t="s">
         <v>5</v>
       </c>
-      <c r="E30" s="138" t="s">
+      <c r="E30" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="F30" s="88">
+      <c r="F30" s="86">
         <v>36</v>
       </c>
       <c r="G30" s="8">
@@ -2112,25 +2300,25 @@
         <f t="shared" si="1"/>
         <v>8550000</v>
       </c>
-      <c r="K30" s="138"/>
-      <c r="L30" s="138"/>
+      <c r="K30" s="94"/>
+      <c r="L30" s="94"/>
       <c r="M30" s="8">
         <f t="shared" si="3"/>
         <v>8550000</v>
       </c>
-      <c r="N30" s="138"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="103"/>
-      <c r="B31" s="139"/>
-      <c r="C31" s="142"/>
-      <c r="D31" s="142" t="s">
+      <c r="N30" s="94"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="164"/>
+      <c r="B31" s="185"/>
+      <c r="C31" s="176"/>
+      <c r="D31" s="176" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="140" t="s">
+      <c r="E31" s="95" t="s">
         <v>16</v>
       </c>
-      <c r="F31" s="89">
+      <c r="F31" s="87">
         <v>36</v>
       </c>
       <c r="G31" s="13">
@@ -2147,47 +2335,200 @@
         <f t="shared" si="1"/>
         <v>8190000</v>
       </c>
-      <c r="K31" s="140"/>
-      <c r="L31" s="140"/>
+      <c r="K31" s="95"/>
+      <c r="L31" s="95"/>
       <c r="M31" s="13">
         <f t="shared" si="3"/>
         <v>8190000</v>
       </c>
-      <c r="N31" s="140"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="93" t="s">
+      <c r="N31" s="95"/>
+    </row>
+    <row r="32" spans="1:16" s="101" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="148">
+        <v>794</v>
+      </c>
+      <c r="B32" s="151">
+        <v>44090</v>
+      </c>
+      <c r="C32" s="145" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="145"/>
+      <c r="E32" s="98" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="98">
+        <v>48</v>
+      </c>
+      <c r="G32" s="99">
+        <v>455000</v>
+      </c>
+      <c r="H32" s="99">
+        <f>F32*G32</f>
+        <v>21840000</v>
+      </c>
+      <c r="I32" s="100">
+        <v>0.5</v>
+      </c>
+      <c r="J32" s="99">
+        <f>H32*(1-I32)</f>
+        <v>10920000</v>
+      </c>
+      <c r="K32" s="93"/>
+      <c r="L32" s="93"/>
+      <c r="M32" s="99">
+        <f>J32</f>
+        <v>10920000</v>
+      </c>
+      <c r="N32" s="99"/>
+      <c r="P32" s="98"/>
+    </row>
+    <row r="33" spans="1:16" s="101" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="149"/>
+      <c r="B33" s="152"/>
+      <c r="C33" s="146"/>
+      <c r="D33" s="146"/>
+      <c r="E33" s="102" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="102">
+        <v>24</v>
+      </c>
+      <c r="G33" s="103">
+        <v>465000</v>
+      </c>
+      <c r="H33" s="103">
+        <f>F33*G33</f>
+        <v>11160000</v>
+      </c>
+      <c r="I33" s="104">
+        <v>0.5</v>
+      </c>
+      <c r="J33" s="103">
+        <f>H33*(1-I33)</f>
+        <v>5580000</v>
+      </c>
+      <c r="K33" s="94"/>
+      <c r="L33" s="94"/>
+      <c r="M33" s="103">
+        <f>J33</f>
+        <v>5580000</v>
+      </c>
+      <c r="N33" s="103"/>
+      <c r="P33" s="102"/>
+    </row>
+    <row r="34" spans="1:16" s="101" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="150"/>
+      <c r="B34" s="153"/>
+      <c r="C34" s="147"/>
+      <c r="D34" s="147"/>
+      <c r="E34" s="105" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="105">
+        <v>24</v>
+      </c>
+      <c r="G34" s="106">
+        <v>485000</v>
+      </c>
+      <c r="H34" s="106">
+        <f>F34*G34</f>
+        <v>11640000</v>
+      </c>
+      <c r="I34" s="107">
+        <v>0.5</v>
+      </c>
+      <c r="J34" s="108">
+        <f>H34*(1-I34)</f>
+        <v>5820000</v>
+      </c>
+      <c r="K34" s="134"/>
+      <c r="L34" s="134"/>
+      <c r="M34" s="106">
+        <f>J34</f>
+        <v>5820000</v>
+      </c>
+      <c r="N34" s="106"/>
+      <c r="P34" s="105"/>
+    </row>
+    <row r="35" spans="1:16" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="109">
+        <v>675</v>
+      </c>
+      <c r="B35" s="110">
+        <v>44096</v>
+      </c>
+      <c r="C35" s="109" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="109"/>
+      <c r="E35" s="111" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" s="111">
+        <v>12</v>
+      </c>
+      <c r="G35" s="112">
+        <v>455000</v>
+      </c>
+      <c r="H35" s="112">
+        <f>F35*G35</f>
+        <v>5460000</v>
+      </c>
+      <c r="I35" s="113">
+        <v>0.5</v>
+      </c>
+      <c r="J35" s="112">
+        <f>H35*(1-I35)</f>
+        <v>2730000</v>
+      </c>
+      <c r="K35" s="135"/>
+      <c r="L35" s="135"/>
+      <c r="M35" s="112">
+        <f>J35</f>
+        <v>2730000</v>
+      </c>
+      <c r="N35" s="112"/>
+      <c r="P35" s="114"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="154" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="94"/>
-      <c r="C32" s="94"/>
-      <c r="D32" s="94"/>
-      <c r="E32" s="95"/>
-      <c r="F32" s="65">
-        <f>SUM(F7:F31)</f>
-        <v>948</v>
-      </c>
-      <c r="G32" s="65"/>
-      <c r="H32" s="66">
-        <f>SUM(H7:H31)</f>
-        <v>418380000</v>
-      </c>
-      <c r="I32" s="65"/>
-      <c r="J32" s="66">
-        <f>SUM(J7:J31)</f>
-        <v>209190000</v>
-      </c>
-      <c r="K32" s="65"/>
-      <c r="L32" s="65"/>
-      <c r="M32" s="55">
-        <f>J32</f>
-        <v>209190000</v>
-      </c>
-      <c r="N32" s="65"/>
+      <c r="B36" s="155"/>
+      <c r="C36" s="155"/>
+      <c r="D36" s="155"/>
+      <c r="E36" s="156"/>
+      <c r="F36" s="64">
+        <f>SUM(F7:F35)</f>
+        <v>1056</v>
+      </c>
+      <c r="G36" s="64"/>
+      <c r="H36" s="65">
+        <f>SUM(H7:H35)</f>
+        <v>468480000</v>
+      </c>
+      <c r="I36" s="64"/>
+      <c r="J36" s="65">
+        <f>SUM(J7:J35)</f>
+        <v>234240000</v>
+      </c>
+      <c r="K36" s="64"/>
+      <c r="L36" s="64"/>
+      <c r="M36" s="54">
+        <f>J36</f>
+        <v>234240000</v>
+      </c>
+      <c r="N36" s="64"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H38" s="144">
+        <f>H36/2</f>
+        <v>234240000</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="D23:D24"/>
+  <mergeCells count="37">
     <mergeCell ref="A28:A31"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="C28:C31"/>
@@ -2204,7 +2545,14 @@
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="D17:D21"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
     <mergeCell ref="E5:I5"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="K5:M5"/>
@@ -2213,13 +2561,11 @@
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="D15:D16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="B17:B21"/>
-    <mergeCell ref="C17:C21"/>
-    <mergeCell ref="D17:D21"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="A36:E36"/>
   </mergeCells>
   <pageMargins left="0.28999999999999998" right="0.2" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2228,139 +2574,139 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="59" customWidth="1"/>
-    <col min="2" max="2" width="12" style="59" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="59" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="59"/>
-    <col min="5" max="5" width="9.28515625" style="59" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="59"/>
-    <col min="7" max="7" width="14" style="59" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" style="59" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" style="59" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" style="59" customWidth="1"/>
-    <col min="11" max="11" width="4.28515625" style="59" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" style="59" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="59"/>
+    <col min="1" max="1" width="6.42578125" style="58" customWidth="1"/>
+    <col min="2" max="2" width="12" style="58" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="58" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="58"/>
+    <col min="5" max="5" width="9.28515625" style="58" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="58" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" style="58" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" style="58" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" style="58" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" style="58" customWidth="1"/>
+    <col min="11" max="11" width="5" style="58" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" style="58" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="58"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="58"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="57"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="57"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="56"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="63"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="62"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="62"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="61"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63"/>
     </row>
     <row r="3" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="114" t="s">
+      <c r="A3" s="177" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="114"/>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114"/>
-      <c r="H3" s="114"/>
-      <c r="I3" s="114"/>
-      <c r="J3" s="114"/>
-      <c r="K3" s="114"/>
-      <c r="L3" s="114"/>
-      <c r="M3" s="114"/>
-      <c r="N3" s="114"/>
-      <c r="O3" s="114"/>
-    </row>
-    <row r="6" spans="1:15" s="67" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="127" t="s">
+      <c r="B3" s="177"/>
+      <c r="C3" s="177"/>
+      <c r="D3" s="177"/>
+      <c r="E3" s="177"/>
+      <c r="F3" s="177"/>
+      <c r="G3" s="177"/>
+      <c r="H3" s="177"/>
+      <c r="I3" s="177"/>
+      <c r="J3" s="177"/>
+      <c r="K3" s="177"/>
+      <c r="L3" s="177"/>
+      <c r="M3" s="177"/>
+      <c r="N3" s="177"/>
+      <c r="O3" s="177"/>
+    </row>
+    <row r="6" spans="1:15" s="66" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="203" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="128" t="s">
+      <c r="B6" s="204" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="133" t="s">
+      <c r="C6" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="125" t="s">
+      <c r="D6" s="195" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="125"/>
-      <c r="F6" s="125"/>
-      <c r="G6" s="125"/>
-      <c r="H6" s="129"/>
-      <c r="I6" s="130" t="s">
+      <c r="E6" s="195"/>
+      <c r="F6" s="195"/>
+      <c r="G6" s="195"/>
+      <c r="H6" s="197"/>
+      <c r="I6" s="198" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="125" t="s">
+      <c r="J6" s="195" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="125"/>
-      <c r="L6" s="125"/>
-      <c r="M6" s="126" t="s">
+      <c r="K6" s="195"/>
+      <c r="L6" s="195"/>
+      <c r="M6" s="196" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="67" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="127"/>
-      <c r="B7" s="128"/>
-      <c r="C7" s="134"/>
-      <c r="D7" s="51" t="s">
+    <row r="7" spans="1:15" s="66" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="203"/>
+      <c r="B7" s="204"/>
+      <c r="C7" s="202"/>
+      <c r="D7" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="51" t="s">
+      <c r="E7" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="52" t="s">
+      <c r="F7" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="53" t="s">
+      <c r="G7" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="54" t="s">
+      <c r="H7" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="130"/>
-      <c r="J7" s="51" t="s">
+      <c r="I7" s="198"/>
+      <c r="J7" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="K7" s="51" t="s">
+      <c r="K7" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="L7" s="51" t="s">
+      <c r="L7" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="M7" s="126"/>
-    </row>
-    <row r="8" spans="1:15" s="67" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M7" s="196"/>
+    </row>
+    <row r="8" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>584</v>
       </c>
@@ -2392,13 +2738,13 @@
       </c>
       <c r="J8" s="26"/>
       <c r="K8" s="26"/>
-      <c r="L8" s="50">
+      <c r="L8" s="49">
         <f>I8</f>
         <v>2730000</v>
       </c>
       <c r="M8" s="30"/>
     </row>
-    <row r="9" spans="1:15" s="67" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>482</v>
       </c>
@@ -2430,20 +2776,20 @@
       </c>
       <c r="J9" s="26"/>
       <c r="K9" s="26"/>
-      <c r="L9" s="50">
+      <c r="L9" s="49">
         <f t="shared" ref="L9:L27" si="2">I9</f>
         <v>450000</v>
       </c>
       <c r="M9" s="30"/>
     </row>
-    <row r="10" spans="1:15" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="102">
+    <row r="10" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="163">
         <v>480</v>
       </c>
-      <c r="B10" s="104">
+      <c r="B10" s="165">
         <v>43998</v>
       </c>
-      <c r="C10" s="122" t="s">
+      <c r="C10" s="192" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="31" t="s">
@@ -2468,16 +2814,16 @@
       </c>
       <c r="J10" s="31"/>
       <c r="K10" s="31"/>
-      <c r="L10" s="50">
+      <c r="L10" s="49">
         <f t="shared" si="2"/>
         <v>2700000</v>
       </c>
       <c r="M10" s="34"/>
     </row>
-    <row r="11" spans="1:15" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="110"/>
-      <c r="B11" s="111"/>
-      <c r="C11" s="123"/>
+    <row r="11" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="171"/>
+      <c r="B11" s="172"/>
+      <c r="C11" s="193"/>
       <c r="D11" s="35" t="s">
         <v>7</v>
       </c>
@@ -2500,16 +2846,16 @@
       </c>
       <c r="J11" s="35"/>
       <c r="K11" s="35"/>
-      <c r="L11" s="50">
+      <c r="L11" s="49">
         <f t="shared" si="2"/>
         <v>5005000</v>
       </c>
       <c r="M11" s="35"/>
     </row>
-    <row r="12" spans="1:15" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="110"/>
-      <c r="B12" s="111"/>
-      <c r="C12" s="123"/>
+    <row r="12" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="171"/>
+      <c r="B12" s="172"/>
+      <c r="C12" s="193"/>
       <c r="D12" s="35" t="s">
         <v>8</v>
       </c>
@@ -2532,7 +2878,7 @@
       </c>
       <c r="J12" s="35"/>
       <c r="K12" s="35"/>
-      <c r="L12" s="50">
+      <c r="L12" s="49">
         <f t="shared" si="2"/>
         <v>2790000</v>
       </c>
@@ -2540,10 +2886,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="110"/>
-      <c r="B13" s="111"/>
-      <c r="C13" s="123"/>
+    <row r="13" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="171"/>
+      <c r="B13" s="172"/>
+      <c r="C13" s="193"/>
       <c r="D13" s="35" t="s">
         <v>14</v>
       </c>
@@ -2566,16 +2912,16 @@
       </c>
       <c r="J13" s="35"/>
       <c r="K13" s="35"/>
-      <c r="L13" s="50">
+      <c r="L13" s="49">
         <f t="shared" si="2"/>
         <v>242500</v>
       </c>
       <c r="M13" s="38"/>
     </row>
-    <row r="14" spans="1:15" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="103"/>
-      <c r="B14" s="105"/>
-      <c r="C14" s="124"/>
+    <row r="14" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="164"/>
+      <c r="B14" s="166"/>
+      <c r="C14" s="194"/>
       <c r="D14" s="39" t="s">
         <v>11</v>
       </c>
@@ -2598,20 +2944,20 @@
       </c>
       <c r="J14" s="39"/>
       <c r="K14" s="39"/>
-      <c r="L14" s="50">
+      <c r="L14" s="49">
         <f t="shared" si="2"/>
         <v>1375000</v>
       </c>
       <c r="M14" s="42"/>
     </row>
-    <row r="15" spans="1:15" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="102">
+    <row r="15" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="163">
         <v>484</v>
       </c>
-      <c r="B15" s="104">
+      <c r="B15" s="165">
         <v>44002</v>
       </c>
-      <c r="C15" s="122" t="s">
+      <c r="C15" s="192" t="s">
         <v>4</v>
       </c>
       <c r="D15" s="31" t="s">
@@ -2636,16 +2982,16 @@
       </c>
       <c r="J15" s="31"/>
       <c r="K15" s="31"/>
-      <c r="L15" s="50">
+      <c r="L15" s="49">
         <f t="shared" si="2"/>
         <v>242500</v>
       </c>
       <c r="M15" s="34"/>
     </row>
-    <row r="16" spans="1:15" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="103"/>
-      <c r="B16" s="105"/>
-      <c r="C16" s="124"/>
+    <row r="16" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="164"/>
+      <c r="B16" s="166"/>
+      <c r="C16" s="194"/>
       <c r="D16" s="39" t="s">
         <v>16</v>
       </c>
@@ -2668,58 +3014,58 @@
       </c>
       <c r="J16" s="39"/>
       <c r="K16" s="39"/>
-      <c r="L16" s="50">
+      <c r="L16" s="49">
         <f t="shared" si="2"/>
         <v>227500</v>
       </c>
       <c r="M16" s="42"/>
     </row>
-    <row r="17" spans="1:13" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="43">
+    <row r="17" spans="1:13" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="96">
         <v>1151</v>
       </c>
-      <c r="B17" s="44">
+      <c r="B17" s="43">
         <v>44006</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="45" t="s">
+      <c r="D17" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="45">
+      <c r="E17" s="44">
         <v>24</v>
       </c>
-      <c r="F17" s="47">
+      <c r="F17" s="46">
         <v>485000</v>
       </c>
-      <c r="G17" s="47">
+      <c r="G17" s="46">
         <f>E17*F17</f>
         <v>11640000</v>
       </c>
-      <c r="H17" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="I17" s="49">
+      <c r="H17" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="I17" s="48">
         <f>G17*(1-H17)</f>
         <v>5820000</v>
       </c>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="50">
+      <c r="J17" s="44"/>
+      <c r="K17" s="44"/>
+      <c r="L17" s="49">
         <f t="shared" si="2"/>
         <v>5820000</v>
       </c>
-      <c r="M17" s="46"/>
-    </row>
-    <row r="18" spans="1:13" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="102">
+      <c r="M17" s="45"/>
+    </row>
+    <row r="18" spans="1:13" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="163">
         <v>487</v>
       </c>
-      <c r="B18" s="104">
+      <c r="B18" s="165">
         <v>44009</v>
       </c>
-      <c r="C18" s="122" t="s">
+      <c r="C18" s="192" t="s">
         <v>4</v>
       </c>
       <c r="D18" s="31" t="s">
@@ -2744,16 +3090,16 @@
       </c>
       <c r="J18" s="31"/>
       <c r="K18" s="31"/>
-      <c r="L18" s="50">
+      <c r="L18" s="49">
         <f t="shared" si="2"/>
         <v>697500</v>
       </c>
       <c r="M18" s="34"/>
     </row>
-    <row r="19" spans="1:13" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="103"/>
-      <c r="B19" s="105"/>
-      <c r="C19" s="124"/>
+    <row r="19" spans="1:13" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="164"/>
+      <c r="B19" s="166"/>
+      <c r="C19" s="194"/>
       <c r="D19" s="39" t="s">
         <v>14</v>
       </c>
@@ -2776,20 +3122,20 @@
       </c>
       <c r="J19" s="39"/>
       <c r="K19" s="39"/>
-      <c r="L19" s="50">
+      <c r="L19" s="49">
         <f t="shared" si="2"/>
         <v>727500</v>
       </c>
       <c r="M19" s="42"/>
     </row>
-    <row r="20" spans="1:13" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="102">
+    <row r="20" spans="1:13" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="163">
         <v>492</v>
       </c>
-      <c r="B20" s="104">
+      <c r="B20" s="165">
         <v>44020</v>
       </c>
-      <c r="C20" s="122" t="s">
+      <c r="C20" s="192" t="s">
         <v>4</v>
       </c>
       <c r="D20" s="31" t="s">
@@ -2814,16 +3160,16 @@
       </c>
       <c r="J20" s="31"/>
       <c r="K20" s="31"/>
-      <c r="L20" s="78">
+      <c r="L20" s="76">
         <f t="shared" si="2"/>
         <v>3487500</v>
       </c>
       <c r="M20" s="34"/>
     </row>
-    <row r="21" spans="1:13" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="110"/>
-      <c r="B21" s="111"/>
-      <c r="C21" s="123"/>
+    <row r="21" spans="1:13" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="171"/>
+      <c r="B21" s="172"/>
+      <c r="C21" s="193"/>
       <c r="D21" s="35" t="s">
         <v>7</v>
       </c>
@@ -2846,16 +3192,16 @@
       </c>
       <c r="J21" s="35"/>
       <c r="K21" s="35"/>
-      <c r="L21" s="86">
+      <c r="L21" s="84">
         <f t="shared" si="2"/>
         <v>2730000</v>
       </c>
       <c r="M21" s="38"/>
     </row>
-    <row r="22" spans="1:13" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="110"/>
-      <c r="B22" s="111"/>
-      <c r="C22" s="123"/>
+    <row r="22" spans="1:13" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="171"/>
+      <c r="B22" s="172"/>
+      <c r="C22" s="193"/>
       <c r="D22" s="35" t="s">
         <v>8</v>
       </c>
@@ -2878,16 +3224,16 @@
       </c>
       <c r="J22" s="35"/>
       <c r="K22" s="35"/>
-      <c r="L22" s="86">
+      <c r="L22" s="84">
         <f t="shared" si="2"/>
         <v>2790000</v>
       </c>
       <c r="M22" s="38"/>
     </row>
-    <row r="23" spans="1:13" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="110"/>
-      <c r="B23" s="111"/>
-      <c r="C23" s="123"/>
+    <row r="23" spans="1:13" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="171"/>
+      <c r="B23" s="172"/>
+      <c r="C23" s="193"/>
       <c r="D23" s="35" t="s">
         <v>9</v>
       </c>
@@ -2910,16 +3256,16 @@
       </c>
       <c r="J23" s="35"/>
       <c r="K23" s="35"/>
-      <c r="L23" s="86">
+      <c r="L23" s="84">
         <f t="shared" si="2"/>
         <v>2850000</v>
       </c>
       <c r="M23" s="38"/>
     </row>
-    <row r="24" spans="1:13" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="110"/>
-      <c r="B24" s="111"/>
-      <c r="C24" s="123"/>
+    <row r="24" spans="1:13" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="171"/>
+      <c r="B24" s="172"/>
+      <c r="C24" s="193"/>
       <c r="D24" s="35" t="s">
         <v>10</v>
       </c>
@@ -2942,16 +3288,16 @@
       </c>
       <c r="J24" s="35"/>
       <c r="K24" s="35"/>
-      <c r="L24" s="86">
+      <c r="L24" s="84">
         <f t="shared" si="2"/>
         <v>2910000</v>
       </c>
       <c r="M24" s="38"/>
     </row>
-    <row r="25" spans="1:13" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="110"/>
-      <c r="B25" s="111"/>
-      <c r="C25" s="123"/>
+    <row r="25" spans="1:13" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="171"/>
+      <c r="B25" s="172"/>
+      <c r="C25" s="193"/>
       <c r="D25" s="35" t="s">
         <v>14</v>
       </c>
@@ -2974,16 +3320,16 @@
       </c>
       <c r="J25" s="35"/>
       <c r="K25" s="35"/>
-      <c r="L25" s="86">
+      <c r="L25" s="84">
         <f t="shared" si="2"/>
         <v>2910000</v>
       </c>
       <c r="M25" s="38"/>
     </row>
-    <row r="26" spans="1:13" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="110"/>
-      <c r="B26" s="111"/>
-      <c r="C26" s="123"/>
+    <row r="26" spans="1:13" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="171"/>
+      <c r="B26" s="172"/>
+      <c r="C26" s="193"/>
       <c r="D26" s="35" t="s">
         <v>15</v>
       </c>
@@ -3006,16 +3352,16 @@
       </c>
       <c r="J26" s="35"/>
       <c r="K26" s="35"/>
-      <c r="L26" s="86">
+      <c r="L26" s="84">
         <f t="shared" si="2"/>
         <v>2730000</v>
       </c>
       <c r="M26" s="38"/>
     </row>
-    <row r="27" spans="1:13" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="103"/>
-      <c r="B27" s="105"/>
-      <c r="C27" s="124"/>
+    <row r="27" spans="1:13" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="164"/>
+      <c r="B27" s="166"/>
+      <c r="C27" s="194"/>
       <c r="D27" s="39" t="s">
         <v>16</v>
       </c>
@@ -3038,17 +3384,17 @@
       </c>
       <c r="J27" s="39"/>
       <c r="K27" s="39"/>
-      <c r="L27" s="79">
+      <c r="L27" s="77">
         <f t="shared" si="2"/>
         <v>2730000</v>
       </c>
       <c r="M27" s="42"/>
     </row>
-    <row r="28" spans="1:13" s="77" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <v>496</v>
       </c>
-      <c r="B28" s="76">
+      <c r="B28" s="74">
         <v>44028</v>
       </c>
       <c r="C28" s="26" t="s">
@@ -3074,16 +3420,16 @@
       </c>
       <c r="J28" s="26"/>
       <c r="K28" s="26"/>
-      <c r="L28" s="50">
+      <c r="L28" s="49">
         <v>2137500</v>
       </c>
       <c r="M28" s="30"/>
     </row>
-    <row r="29" spans="1:13" s="77" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
         <v>497</v>
       </c>
-      <c r="B29" s="76">
+      <c r="B29" s="74">
         <v>44029</v>
       </c>
       <c r="C29" s="26" t="s">
@@ -3109,16 +3455,16 @@
       </c>
       <c r="J29" s="26"/>
       <c r="K29" s="26"/>
-      <c r="L29" s="50">
+      <c r="L29" s="49">
         <v>227500</v>
       </c>
       <c r="M29" s="30"/>
     </row>
-    <row r="30" spans="1:13" s="77" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16">
         <v>610</v>
       </c>
-      <c r="B30" s="76">
+      <c r="B30" s="74">
         <v>44031</v>
       </c>
       <c r="C30" s="26" t="s">
@@ -3144,19 +3490,19 @@
       </c>
       <c r="J30" s="26"/>
       <c r="K30" s="26"/>
-      <c r="L30" s="50">
+      <c r="L30" s="49">
         <v>13650000</v>
       </c>
       <c r="M30" s="30"/>
     </row>
-    <row r="31" spans="1:13" s="77" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="102">
+    <row r="31" spans="1:13" s="75" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="163">
         <v>617</v>
       </c>
-      <c r="B31" s="104">
+      <c r="B31" s="165">
         <v>44034</v>
       </c>
-      <c r="C31" s="131" t="s">
+      <c r="C31" s="199" t="s">
         <v>4</v>
       </c>
       <c r="D31" s="31" t="s">
@@ -3179,15 +3525,15 @@
       </c>
       <c r="J31" s="31"/>
       <c r="K31" s="31"/>
-      <c r="L31" s="78">
+      <c r="L31" s="76">
         <v>562500</v>
       </c>
       <c r="M31" s="34"/>
     </row>
-    <row r="32" spans="1:13" s="77" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="103"/>
-      <c r="B32" s="105"/>
-      <c r="C32" s="132"/>
+    <row r="32" spans="1:13" s="75" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="164"/>
+      <c r="B32" s="166"/>
+      <c r="C32" s="200"/>
       <c r="D32" s="39" t="s">
         <v>7</v>
       </c>
@@ -3208,60 +3554,60 @@
       </c>
       <c r="J32" s="39"/>
       <c r="K32" s="39"/>
-      <c r="L32" s="79">
+      <c r="L32" s="77">
         <v>2730000</v>
       </c>
       <c r="M32" s="42"/>
     </row>
-    <row r="33" spans="1:13" s="77" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="68">
+    <row r="33" spans="1:17" s="75" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="97">
         <v>618</v>
       </c>
-      <c r="B33" s="74">
+      <c r="B33" s="72">
         <v>44036</v>
       </c>
-      <c r="C33" s="83" t="s">
+      <c r="C33" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="45" t="s">
+      <c r="D33" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="45">
+      <c r="E33" s="44">
         <v>12</v>
       </c>
-      <c r="F33" s="80">
+      <c r="F33" s="78">
         <v>455000</v>
       </c>
-      <c r="G33" s="80">
+      <c r="G33" s="78">
         <v>5460000</v>
       </c>
-      <c r="H33" s="81">
-        <v>0.5</v>
-      </c>
-      <c r="I33" s="82">
+      <c r="H33" s="79">
+        <v>0.5</v>
+      </c>
+      <c r="I33" s="80">
         <v>2730000</v>
       </c>
-      <c r="J33" s="83"/>
-      <c r="K33" s="83"/>
-      <c r="L33" s="84">
+      <c r="J33" s="81"/>
+      <c r="K33" s="81"/>
+      <c r="L33" s="82">
         <v>2730000</v>
       </c>
-      <c r="M33" s="85"/>
-    </row>
-    <row r="34" spans="1:13" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="102">
+      <c r="M33" s="83"/>
+    </row>
+    <row r="34" spans="1:17" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="163">
         <v>642</v>
       </c>
-      <c r="B34" s="104">
+      <c r="B34" s="165">
         <v>44056</v>
       </c>
-      <c r="C34" s="131" t="s">
+      <c r="C34" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="91" t="s">
+      <c r="D34" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="91">
+      <c r="E34" s="88">
         <v>24</v>
       </c>
       <c r="F34" s="32">
@@ -3276,21 +3622,21 @@
       <c r="I34" s="4">
         <v>2730000</v>
       </c>
-      <c r="J34" s="91"/>
-      <c r="K34" s="91"/>
+      <c r="J34" s="88"/>
+      <c r="K34" s="88"/>
       <c r="L34" s="4">
         <v>2730000</v>
       </c>
       <c r="M34" s="34"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="103"/>
-      <c r="B35" s="105"/>
-      <c r="C35" s="132"/>
-      <c r="D35" s="92" t="s">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" s="164"/>
+      <c r="B35" s="166"/>
+      <c r="C35" s="200"/>
+      <c r="D35" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="E35" s="92">
+      <c r="E35" s="89">
         <v>5</v>
       </c>
       <c r="F35" s="40">
@@ -3305,91 +3651,658 @@
       <c r="I35" s="15">
         <v>2730000</v>
       </c>
-      <c r="J35" s="92"/>
-      <c r="K35" s="92"/>
+      <c r="J35" s="89"/>
+      <c r="K35" s="89"/>
       <c r="L35" s="15">
         <v>2730000</v>
       </c>
       <c r="M35" s="42"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="68">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" s="97">
         <v>767</v>
       </c>
-      <c r="B36" s="74">
+      <c r="B36" s="72">
         <v>44065</v>
       </c>
-      <c r="C36" s="83" t="s">
+      <c r="C36" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="90" t="s">
+      <c r="D36" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="E36" s="90">
+      <c r="E36" s="81">
         <v>12</v>
       </c>
-      <c r="F36" s="80">
+      <c r="F36" s="78">
         <v>485000</v>
       </c>
-      <c r="G36" s="80">
+      <c r="G36" s="78">
         <v>5460000</v>
       </c>
-      <c r="H36" s="81">
-        <v>0.5</v>
-      </c>
-      <c r="I36" s="82">
+      <c r="H36" s="79">
+        <v>0.5</v>
+      </c>
+      <c r="I36" s="80">
         <v>2730000</v>
       </c>
-      <c r="J36" s="83"/>
-      <c r="K36" s="83"/>
-      <c r="L36" s="84">
+      <c r="J36" s="81"/>
+      <c r="K36" s="81"/>
+      <c r="L36" s="82">
         <v>2730000</v>
       </c>
-      <c r="M36" s="85"/>
-    </row>
-    <row r="37" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="120" t="s">
+      <c r="M36" s="140"/>
+    </row>
+    <row r="37" spans="1:17" s="101" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="148">
+        <v>664</v>
+      </c>
+      <c r="B37" s="151">
+        <v>44088</v>
+      </c>
+      <c r="C37" s="187" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="115" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="90">
+        <v>24</v>
+      </c>
+      <c r="F37" s="32">
+        <v>455000</v>
+      </c>
+      <c r="G37" s="116">
+        <f t="shared" ref="G37:G48" si="5">E37*F37</f>
+        <v>10920000</v>
+      </c>
+      <c r="H37" s="117">
+        <v>0.5</v>
+      </c>
+      <c r="I37" s="118">
+        <f>G37*(1-H37)</f>
+        <v>5460000</v>
+      </c>
+      <c r="J37" s="99"/>
+      <c r="K37" s="99"/>
+      <c r="L37" s="119">
+        <f>I37</f>
+        <v>5460000</v>
+      </c>
+      <c r="M37" s="98"/>
+      <c r="Q37" s="120"/>
+    </row>
+    <row r="38" spans="1:17" s="101" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="150"/>
+      <c r="B38" s="153"/>
+      <c r="C38" s="189"/>
+      <c r="D38" s="121" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="92">
+        <v>24</v>
+      </c>
+      <c r="F38" s="40">
+        <v>475000</v>
+      </c>
+      <c r="G38" s="122">
+        <f t="shared" si="5"/>
+        <v>11400000</v>
+      </c>
+      <c r="H38" s="123">
+        <v>0.5</v>
+      </c>
+      <c r="I38" s="108">
+        <f t="shared" ref="I38:I52" si="6">G38*(1-H38)</f>
+        <v>5700000</v>
+      </c>
+      <c r="J38" s="106"/>
+      <c r="K38" s="106"/>
+      <c r="L38" s="124">
+        <f t="shared" ref="L38:L52" si="7">I38</f>
+        <v>5700000</v>
+      </c>
+      <c r="M38" s="105"/>
+      <c r="Q38" s="120"/>
+    </row>
+    <row r="39" spans="1:17" s="101" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="111">
+        <v>666</v>
+      </c>
+      <c r="B39" s="110">
+        <v>44091</v>
+      </c>
+      <c r="C39" s="125" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="126" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="26">
+        <v>42</v>
+      </c>
+      <c r="F39" s="27">
+        <v>455000</v>
+      </c>
+      <c r="G39" s="141">
+        <f t="shared" si="5"/>
+        <v>19110000</v>
+      </c>
+      <c r="H39" s="139">
+        <v>0.5</v>
+      </c>
+      <c r="I39" s="127">
+        <f t="shared" si="6"/>
+        <v>9555000</v>
+      </c>
+      <c r="J39" s="112"/>
+      <c r="K39" s="112"/>
+      <c r="L39" s="128">
+        <f t="shared" si="7"/>
+        <v>9555000</v>
+      </c>
+      <c r="M39" s="111"/>
+      <c r="Q39" s="120"/>
+    </row>
+    <row r="40" spans="1:17" s="101" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="111">
+        <v>669</v>
+      </c>
+      <c r="B40" s="110">
+        <v>44092</v>
+      </c>
+      <c r="C40" s="125" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="126" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="26">
+        <v>24</v>
+      </c>
+      <c r="F40" s="27">
+        <v>225000</v>
+      </c>
+      <c r="G40" s="141">
+        <f t="shared" si="5"/>
+        <v>5400000</v>
+      </c>
+      <c r="H40" s="139">
+        <v>0.5</v>
+      </c>
+      <c r="I40" s="127">
+        <f t="shared" si="6"/>
+        <v>2700000</v>
+      </c>
+      <c r="J40" s="112"/>
+      <c r="K40" s="112"/>
+      <c r="L40" s="128">
+        <f t="shared" si="7"/>
+        <v>2700000</v>
+      </c>
+      <c r="M40" s="111"/>
+      <c r="Q40" s="120"/>
+    </row>
+    <row r="41" spans="1:17" s="101" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="148">
+        <v>677</v>
+      </c>
+      <c r="B41" s="151">
+        <v>44096</v>
+      </c>
+      <c r="C41" s="187" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="115" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="90">
+        <v>1</v>
+      </c>
+      <c r="F41" s="32">
+        <v>225000</v>
+      </c>
+      <c r="G41" s="116">
+        <f t="shared" si="5"/>
+        <v>225000</v>
+      </c>
+      <c r="H41" s="117">
+        <v>0.5</v>
+      </c>
+      <c r="I41" s="118">
+        <f t="shared" si="6"/>
+        <v>112500</v>
+      </c>
+      <c r="J41" s="99"/>
+      <c r="K41" s="99"/>
+      <c r="L41" s="119">
+        <f t="shared" si="7"/>
+        <v>112500</v>
+      </c>
+      <c r="M41" s="98"/>
+      <c r="Q41" s="120"/>
+    </row>
+    <row r="42" spans="1:17" s="101" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="149"/>
+      <c r="B42" s="152"/>
+      <c r="C42" s="188"/>
+      <c r="D42" s="129" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="91">
+        <v>1</v>
+      </c>
+      <c r="F42" s="36">
+        <v>455000</v>
+      </c>
+      <c r="G42" s="142">
+        <f t="shared" si="5"/>
+        <v>455000</v>
+      </c>
+      <c r="H42" s="136">
+        <v>0.5</v>
+      </c>
+      <c r="I42" s="137">
+        <f t="shared" si="6"/>
+        <v>227500</v>
+      </c>
+      <c r="J42" s="103"/>
+      <c r="K42" s="103"/>
+      <c r="L42" s="138">
+        <f t="shared" si="7"/>
+        <v>227500</v>
+      </c>
+      <c r="M42" s="102"/>
+      <c r="Q42" s="120"/>
+    </row>
+    <row r="43" spans="1:17" s="101" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="149"/>
+      <c r="B43" s="152"/>
+      <c r="C43" s="188"/>
+      <c r="D43" s="129" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="91">
+        <v>1</v>
+      </c>
+      <c r="F43" s="36">
+        <v>465000</v>
+      </c>
+      <c r="G43" s="142">
+        <f t="shared" si="5"/>
+        <v>465000</v>
+      </c>
+      <c r="H43" s="136">
+        <v>0.5</v>
+      </c>
+      <c r="I43" s="137">
+        <f t="shared" si="6"/>
+        <v>232500</v>
+      </c>
+      <c r="J43" s="103"/>
+      <c r="K43" s="103"/>
+      <c r="L43" s="138">
+        <f t="shared" si="7"/>
+        <v>232500</v>
+      </c>
+      <c r="M43" s="102"/>
+      <c r="Q43" s="120"/>
+    </row>
+    <row r="44" spans="1:17" s="101" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="149"/>
+      <c r="B44" s="152"/>
+      <c r="C44" s="188"/>
+      <c r="D44" s="129" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="91">
+        <v>1</v>
+      </c>
+      <c r="F44" s="36">
+        <v>475000</v>
+      </c>
+      <c r="G44" s="142">
+        <f t="shared" si="5"/>
+        <v>475000</v>
+      </c>
+      <c r="H44" s="136">
+        <v>0.5</v>
+      </c>
+      <c r="I44" s="137">
+        <f t="shared" si="6"/>
+        <v>237500</v>
+      </c>
+      <c r="J44" s="103"/>
+      <c r="K44" s="103"/>
+      <c r="L44" s="138">
+        <f t="shared" si="7"/>
+        <v>237500</v>
+      </c>
+      <c r="M44" s="102"/>
+      <c r="Q44" s="120"/>
+    </row>
+    <row r="45" spans="1:17" s="101" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="149"/>
+      <c r="B45" s="152"/>
+      <c r="C45" s="188"/>
+      <c r="D45" s="129" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" s="91">
+        <v>1</v>
+      </c>
+      <c r="F45" s="36">
+        <v>485000</v>
+      </c>
+      <c r="G45" s="142">
+        <f t="shared" si="5"/>
+        <v>485000</v>
+      </c>
+      <c r="H45" s="136">
+        <v>0.5</v>
+      </c>
+      <c r="I45" s="137">
+        <f t="shared" si="6"/>
+        <v>242500</v>
+      </c>
+      <c r="J45" s="103"/>
+      <c r="K45" s="103"/>
+      <c r="L45" s="138">
+        <f t="shared" si="7"/>
+        <v>242500</v>
+      </c>
+      <c r="M45" s="131"/>
+      <c r="Q45" s="120"/>
+    </row>
+    <row r="46" spans="1:17" s="132" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="149"/>
+      <c r="B46" s="152"/>
+      <c r="C46" s="188"/>
+      <c r="D46" s="129" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46" s="91">
+        <v>1</v>
+      </c>
+      <c r="F46" s="36">
+        <v>485000</v>
+      </c>
+      <c r="G46" s="142">
+        <f t="shared" si="5"/>
+        <v>485000</v>
+      </c>
+      <c r="H46" s="136">
+        <v>0.5</v>
+      </c>
+      <c r="I46" s="137">
+        <f t="shared" si="6"/>
+        <v>242500</v>
+      </c>
+      <c r="J46" s="130"/>
+      <c r="K46" s="130"/>
+      <c r="L46" s="138">
+        <f t="shared" si="7"/>
+        <v>242500</v>
+      </c>
+      <c r="M46" s="131"/>
+    </row>
+    <row r="47" spans="1:17" s="132" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="149"/>
+      <c r="B47" s="152"/>
+      <c r="C47" s="188"/>
+      <c r="D47" s="129" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" s="91">
+        <v>1</v>
+      </c>
+      <c r="F47" s="36">
+        <v>455000</v>
+      </c>
+      <c r="G47" s="142">
+        <f t="shared" si="5"/>
+        <v>455000</v>
+      </c>
+      <c r="H47" s="136">
+        <v>0.5</v>
+      </c>
+      <c r="I47" s="137">
+        <f t="shared" si="6"/>
+        <v>227500</v>
+      </c>
+      <c r="J47" s="130"/>
+      <c r="K47" s="130"/>
+      <c r="L47" s="138">
+        <f t="shared" si="7"/>
+        <v>227500</v>
+      </c>
+      <c r="M47" s="131"/>
+    </row>
+    <row r="48" spans="1:17" s="132" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="150"/>
+      <c r="B48" s="153"/>
+      <c r="C48" s="189"/>
+      <c r="D48" s="121" t="s">
+        <v>16</v>
+      </c>
+      <c r="E48" s="92">
+        <v>1</v>
+      </c>
+      <c r="F48" s="40">
+        <v>455000</v>
+      </c>
+      <c r="G48" s="122">
+        <f t="shared" si="5"/>
+        <v>455000</v>
+      </c>
+      <c r="H48" s="123">
+        <v>0.5</v>
+      </c>
+      <c r="I48" s="108">
+        <f t="shared" si="6"/>
+        <v>227500</v>
+      </c>
+      <c r="J48" s="124"/>
+      <c r="K48" s="133"/>
+      <c r="L48" s="124">
+        <f t="shared" si="7"/>
+        <v>227500</v>
+      </c>
+      <c r="M48" s="95"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="163">
+        <v>809</v>
+      </c>
+      <c r="B49" s="151">
+        <v>44107</v>
+      </c>
+      <c r="C49" s="148" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="93" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" s="90">
+        <v>23</v>
+      </c>
+      <c r="F49" s="32">
+        <v>225000</v>
+      </c>
+      <c r="G49" s="116">
+        <f t="shared" ref="G49:G52" si="8">E49*F49</f>
+        <v>5175000</v>
+      </c>
+      <c r="H49" s="117">
+        <v>0.5</v>
+      </c>
+      <c r="I49" s="118">
+        <f t="shared" si="6"/>
+        <v>2587500</v>
+      </c>
+      <c r="J49" s="93"/>
+      <c r="K49" s="93"/>
+      <c r="L49" s="119">
+        <f t="shared" si="7"/>
+        <v>2587500</v>
+      </c>
+      <c r="M49" s="119"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="171"/>
+      <c r="B50" s="152"/>
+      <c r="C50" s="149"/>
+      <c r="D50" s="94" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="91">
+        <v>8</v>
+      </c>
+      <c r="F50" s="36">
+        <v>455000</v>
+      </c>
+      <c r="G50" s="142">
+        <f t="shared" si="8"/>
+        <v>3640000</v>
+      </c>
+      <c r="H50" s="136">
+        <v>0.5</v>
+      </c>
+      <c r="I50" s="137">
+        <f t="shared" si="6"/>
+        <v>1820000</v>
+      </c>
+      <c r="J50" s="94"/>
+      <c r="K50" s="94"/>
+      <c r="L50" s="138">
+        <f t="shared" si="7"/>
+        <v>1820000</v>
+      </c>
+      <c r="M50" s="138"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="164"/>
+      <c r="B51" s="153"/>
+      <c r="C51" s="150"/>
+      <c r="D51" s="95" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" s="92">
+        <v>12</v>
+      </c>
+      <c r="F51" s="40">
+        <v>485000</v>
+      </c>
+      <c r="G51" s="122">
+        <f t="shared" si="8"/>
+        <v>5820000</v>
+      </c>
+      <c r="H51" s="123">
+        <v>0.5</v>
+      </c>
+      <c r="I51" s="108">
+        <f t="shared" si="6"/>
+        <v>2910000</v>
+      </c>
+      <c r="J51" s="95"/>
+      <c r="K51" s="95"/>
+      <c r="L51" s="124">
+        <f t="shared" si="7"/>
+        <v>2910000</v>
+      </c>
+      <c r="M51" s="124"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="16">
+        <v>810</v>
+      </c>
+      <c r="B52" s="110">
+        <v>44109</v>
+      </c>
+      <c r="C52" s="135"/>
+      <c r="D52" s="135" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="26">
+        <v>36</v>
+      </c>
+      <c r="F52" s="27">
+        <v>485000</v>
+      </c>
+      <c r="G52" s="122">
+        <f t="shared" si="8"/>
+        <v>17460000</v>
+      </c>
+      <c r="H52" s="139">
+        <v>0.5</v>
+      </c>
+      <c r="I52" s="127">
+        <f t="shared" si="6"/>
+        <v>8730000</v>
+      </c>
+      <c r="J52" s="135"/>
+      <c r="K52" s="135"/>
+      <c r="L52" s="128">
+        <f t="shared" si="7"/>
+        <v>8730000</v>
+      </c>
+      <c r="M52" s="128"/>
+    </row>
+    <row r="53" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="190" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="121"/>
-      <c r="C37" s="121"/>
-      <c r="D37" s="69"/>
-      <c r="E37" s="69">
-        <f>SUM(E8:E36)</f>
-        <v>367</v>
-      </c>
-      <c r="F37" s="69"/>
-      <c r="G37" s="70">
-        <f>SUM(G8:G36)</f>
-        <v>152745000</v>
-      </c>
-      <c r="H37" s="69"/>
-      <c r="I37" s="71">
-        <f>SUM(I8:I36)</f>
-        <v>76372500</v>
-      </c>
-      <c r="J37" s="69"/>
-      <c r="K37" s="69"/>
-      <c r="L37" s="72">
-        <f>I37</f>
-        <v>76372500</v>
-      </c>
-      <c r="M37" s="69"/>
+      <c r="B53" s="191"/>
+      <c r="C53" s="191"/>
+      <c r="D53" s="67"/>
+      <c r="E53" s="67">
+        <f>SUM(E8:E52)</f>
+        <v>568</v>
+      </c>
+      <c r="F53" s="67"/>
+      <c r="G53" s="68">
+        <f>SUM(G8:G52)</f>
+        <v>235170000</v>
+      </c>
+      <c r="H53" s="67"/>
+      <c r="I53" s="69">
+        <f>SUM(I8:I52)</f>
+        <v>117585000</v>
+      </c>
+      <c r="J53" s="67"/>
+      <c r="K53" s="67"/>
+      <c r="L53" s="70">
+        <f>I53</f>
+        <v>117585000</v>
+      </c>
+      <c r="M53" s="67"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G55" s="143">
+        <f>G53/2</f>
+        <v>117585000</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="36">
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="C6:C7"/>
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="C34:C35"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="C10:C14"/>
     <mergeCell ref="D6:H6"/>
     <mergeCell ref="I6:I7"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="A53:C53"/>
     <mergeCell ref="A3:O3"/>
     <mergeCell ref="A20:A27"/>
     <mergeCell ref="B20:B27"/>
@@ -3402,11 +4315,14 @@
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="J6:L6"/>
     <mergeCell ref="M6:M7"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="C10:C14"/>
+    <mergeCell ref="A41:A48"/>
+    <mergeCell ref="B41:B48"/>
+    <mergeCell ref="C41:C48"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="C49:C51"/>
   </mergeCells>
   <pageMargins left="0.41" right="0.39" top="0.37" bottom="0.37" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>